<commit_message>
Raport medyczny dla groupm i wewn działa.
</commit_message>
<xml_diff>
--- a/Doc/Samples/Raporty/Medicover/medicover luty 2014 ela.xlsx
+++ b/Doc/Samples/Raporty/Medicover/medicover luty 2014 ela.xlsx
@@ -1504,14 +1504,14 @@
   <sheetPr codeName="Arkusz1" filterMode="1"/>
   <dimension ref="A1:N198"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U151" sqref="U151"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
     <col min="1" max="1" width="5.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="4.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.875" style="2" customWidth="1"/>
     <col min="3" max="3" width="26.75" style="4" customWidth="1"/>
     <col min="4" max="4" width="21.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.125" style="3" customWidth="1"/>

</xml_diff>